<commit_message>
change fig3 to one
</commit_message>
<xml_diff>
--- a/class_authorNum.xlsx
+++ b/class_authorNum.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -394,11 +394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="178799360"/>
-        <c:axId val="178800896"/>
+        <c:axId val="178414456"/>
+        <c:axId val="178412888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="178799360"/>
+        <c:axId val="178414456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,7 +463,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178800896"/>
+        <c:crossAx val="178412888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -471,7 +471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178800896"/>
+        <c:axId val="178412888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +546,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178799360"/>
+        <c:crossAx val="178414456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -595,562 +595,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1187,7 +631,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1229,7 +673,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1264,7 +708,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1475,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>